<commit_message>
Updating Sprint 5 Backlog per completion
-Sprint 5 Backlog updated
</commit_message>
<xml_diff>
--- a/sprints/sprint 5/Sprint 5 Backlog.xlsx
+++ b/sprints/sprint 5/Sprint 5 Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="43">
   <si>
     <t>Task</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Estimate (hrs)</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -43,12 +40,12 @@
     <t>Brandon</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t>Create Interface for Database functionality.</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Create class implementing Interface fucntionality. (two constructors)</t>
   </si>
   <si>
@@ -67,16 +64,10 @@
     <t>Fix updating rentals.</t>
   </si>
   <si>
-    <t>Refactor employee history to use the new view.</t>
-  </si>
-  <si>
-    <t>Add seperate view for employee history that highlights the action and not the rental.</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>Brandon/Caleb</t>
+    <t>Refactor employee history to show rental action first.</t>
+  </si>
+  <si>
+    <t>Refactor employee history to show actions first</t>
   </si>
   <si>
     <t>Warehouse Web</t>
@@ -149,12 +140,6 @@
   </si>
   <si>
     <t>Update Unit Testing for new Controller behavior</t>
-  </si>
-  <si>
-    <t>Done-ish</t>
-  </si>
-  <si>
-    <t>Need to test more cases, Coverage is at its highest</t>
   </si>
 </sst>
 </file>
@@ -183,20 +168,18 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font/>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
     </font>
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
       <color rgb="FF24292E"/>
@@ -223,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -239,26 +222,29 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -485,7 +471,6 @@
     <col customWidth="1" min="3" max="3" width="14.71"/>
     <col customWidth="1" min="4" max="4" width="10.43"/>
     <col customWidth="1" min="5" max="5" width="13.29"/>
-    <col customWidth="1" min="6" max="6" width="40.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -507,23 +492,26 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" s="6">
-        <v>6.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="F2" s="7">
+        <f>SUM(E1:E10)</f>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -531,266 +519,296 @@
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="9">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="9">
         <v>3.0</v>
-      </c>
-      <c r="G4" s="7">
-        <f>SUM(E1:E11)</f>
-        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6">
-        <v>4.0</v>
+      <c r="D5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9">
+        <v>6.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6">
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9">
         <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6">
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="9">
         <v>3.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="E8" s="6">
         <v>6.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6">
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="9">
         <v>2.0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
+    <row r="11">
+      <c r="A11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6">
-        <v>1.0</v>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="F11" s="7">
+        <f>SUM(E11:E18)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="9">
         <v>3.0</v>
-      </c>
-      <c r="G12" s="7">
-        <f>SUM(E11:E19)</f>
-        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9">
         <v>3.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6">
-        <v>3.0</v>
+        <v>20</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="9">
+        <v>4.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6">
+        <v>20</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="9">
         <v>4.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6">
+        <v>20</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="9">
         <v>4.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6">
-        <v>4.0</v>
+        <v>20</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="9">
+        <v>6.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6">
-        <v>6.0</v>
+        <v>20</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="9">
+        <v>2.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6">
-        <v>2.0</v>
+        <v>30</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="F19" s="7">
+        <f>SUM(E19:E31)</f>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
@@ -798,419 +816,395 @@
         <v>31</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="6">
-        <v>5.0</v>
+        <v>30</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9">
+        <v>2.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="9">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="9">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="6">
+      <c r="B23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="9">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="9">
         <v>2.0</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="6">
+    <row r="28">
+      <c r="A28" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="9">
         <v>2.0</v>
-      </c>
-      <c r="G22" s="7">
-        <f>SUM(E20:E32)</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="6">
-        <v>1.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="6">
-        <v>2.0</v>
+        <v>9</v>
+      </c>
+      <c r="E31" s="9">
+        <v>6.0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33">
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
+      <c r="A33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34">
-      <c r="A34" s="12"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="6"/>
+      <c r="A34" s="13"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35">
-      <c r="A35" s="12"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="6"/>
+      <c r="A35" s="13"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36">
-      <c r="A36" s="12"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="6"/>
+      <c r="A36" s="13"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37">
-      <c r="A37" s="12"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="6"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38">
-      <c r="D38" s="5"/>
-      <c r="E38" s="6"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="39">
-      <c r="D39" s="5"/>
-      <c r="E39" s="6"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40">
-      <c r="D40" s="5"/>
-      <c r="E40" s="6"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9"/>
     </row>
     <row r="41">
-      <c r="D41" s="5"/>
-      <c r="E41" s="6"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42">
-      <c r="D42" s="5"/>
-      <c r="E42" s="6"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43">
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44">
-      <c r="D44" s="5"/>
-      <c r="E44" s="6"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45">
-      <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="9"/>
     </row>
     <row r="46">
-      <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="47">
-      <c r="D47" s="5"/>
-      <c r="E47" s="6"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
     </row>
     <row r="48">
-      <c r="D48" s="5"/>
-      <c r="E48" s="6"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="49">
-      <c r="E49" s="6"/>
+      <c r="E49" s="9"/>
     </row>
     <row r="50">
-      <c r="E50" s="6"/>
+      <c r="E50" s="9"/>
     </row>
     <row r="51">
-      <c r="E51" s="6"/>
+      <c r="E51" s="9"/>
     </row>
     <row r="52">
-      <c r="E52" s="6"/>
+      <c r="A52" s="13"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53">
-      <c r="A53" s="12"/>
-      <c r="E53" s="6"/>
+      <c r="A53" s="13"/>
+      <c r="E53" s="9"/>
     </row>
     <row r="54">
-      <c r="A54" s="12"/>
-      <c r="E54" s="6"/>
+      <c r="A54" s="13"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="55">
-      <c r="A55" s="12"/>
-      <c r="E55" s="6"/>
+      <c r="A55" s="13"/>
+      <c r="E55" s="9"/>
     </row>
     <row r="56">
-      <c r="A56" s="12"/>
-      <c r="E56" s="6"/>
+      <c r="A56" s="11"/>
+      <c r="E56" s="9"/>
     </row>
     <row r="57">
-      <c r="A57" s="8"/>
-      <c r="E57" s="6"/>
+      <c r="E57" s="9"/>
     </row>
     <row r="58">
-      <c r="E58" s="6"/>
+      <c r="E58" s="9"/>
     </row>
     <row r="59">
-      <c r="E59" s="6"/>
+      <c r="E59" s="9"/>
     </row>
     <row r="60">
-      <c r="E60" s="6"/>
+      <c r="E60" s="9"/>
     </row>
     <row r="61">
-      <c r="E61" s="6"/>
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="E61" s="9"/>
     </row>
     <row r="62">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="E62" s="6"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="E62" s="9"/>
     </row>
     <row r="63">
-      <c r="A63" s="13"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="E63" s="6"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="E63" s="9"/>
     </row>
     <row r="64">
-      <c r="A64" s="8"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="E64" s="6"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="E64" s="9"/>
     </row>
     <row r="65">
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="E65" s="6"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="E65" s="9"/>
     </row>
     <row r="66">
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="E66" s="6"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="E66" s="9"/>
     </row>
     <row r="67">
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="E67" s="6"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="E67" s="9"/>
     </row>
     <row r="68">
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="E68" s="6"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="E68" s="9"/>
     </row>
     <row r="69">
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="E69" s="6"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="E69" s="9"/>
     </row>
     <row r="70">
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="E70" s="6"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="E70" s="9"/>
     </row>
     <row r="71">
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="E71" s="6"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="E71" s="9"/>
     </row>
     <row r="72">
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="E72" s="6"/>
+      <c r="E72" s="9"/>
     </row>
     <row r="73">
-      <c r="E73" s="6"/>
+      <c r="A73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="9"/>
     </row>
     <row r="74">
-      <c r="A74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="6"/>
+      <c r="A74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="9"/>
     </row>
     <row r="75">
-      <c r="A75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="6"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="9"/>
     </row>
     <row r="76">
-      <c r="D76" s="8"/>
-      <c r="E76" s="6"/>
-    </row>
-    <row r="77">
-      <c r="D77" s="8"/>
-      <c r="E77" s="6"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="9"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>